<commit_message>
New and modified Data
</commit_message>
<xml_diff>
--- a/excel_sheets/debt_ceiling_tz.xlsx
+++ b/excel_sheets/debt_ceiling_tz.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\OneDrive\Documents\GitHub\Stock_Markets\excel_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A148E647-1857-4476-A3E9-0B240BF144DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC7964E-8695-4D56-9D9F-D19526AE4633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E8AB2C62-67C0-4743-AC00-3531686E0223}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="52">
   <si>
     <t>dates</t>
   </si>
@@ -110,11 +110,6 @@
     <t>112-25</t>
   </si>
   <si>
-    <t xml:space="preserve">Located at Title 3, Sec. 301-1A subsection(a); 
-if the Treasury exercises the suthority to borrow an 
-additional 900B dollars, debt limit is rasied by 400B(August 2011) and if disapproval committee has lapsed discusssions debt limit is raised an additional 500B (Septmber 2011) </t>
-  </si>
-  <si>
     <t>Located at Title 3, Sec. 301-1A subsection(a);
 In the event that debt is within 100B of the limit and further borrowing is required, it would induce a 1.2T dollar increase to the limit and has to pass joint disapproval committee</t>
   </si>
@@ -201,6 +196,11 @@
   </si>
   <si>
     <t xml:space="preserve">Located at Division D, Sec.401; debt limit is suspended from June 3, 2023 to Jan 1, 2025 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Located at Title 3, Sec. 301-1A subsection(a); 
+if the Treasury exercises the authority to borrow an 
+additional 900B dollars, debt limit is raised by 400B(August 2011) and if disapproval committee has lapsed discusssions debt limit is raised an additional 500B (Septmber 2011) </t>
   </si>
 </sst>
 </file>
@@ -208,7 +208,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -247,7 +247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -266,9 +266,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -306,7 +306,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -412,7 +412,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -554,7 +554,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -565,7 +565,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +776,7 @@
         <v>22</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
         <v>19</v>
@@ -793,7 +793,7 @@
         <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
         <v>19</v>
@@ -810,7 +810,7 @@
         <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
         <v>19</v>
@@ -821,13 +821,13 @@
         <v>41309</v>
       </c>
       <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
@@ -841,10 +841,10 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="E16" t="s">
         <v>19</v>
@@ -855,13 +855,13 @@
         <v>41564</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
@@ -875,10 +875,10 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="E18" t="s">
         <v>19</v>
@@ -889,13 +889,13 @@
         <v>41685</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="E19" t="s">
         <v>19</v>
@@ -909,10 +909,10 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="E20" t="s">
         <v>19</v>
@@ -923,13 +923,13 @@
         <v>42310</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E21" t="s">
         <v>19</v>
@@ -943,10 +943,10 @@
         <v>14</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -954,16 +954,16 @@
         <v>42986</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -974,10 +974,10 @@
         <v>14</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -985,16 +985,16 @@
         <v>43140</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1005,10 +1005,10 @@
         <v>14</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1016,16 +1016,16 @@
         <v>43679</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1035,11 +1035,14 @@
       <c r="B28" t="s">
         <v>14</v>
       </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
       <c r="D28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1050,13 +1053,13 @@
         <v>14</v>
       </c>
       <c r="C29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" t="s">
         <v>44</v>
       </c>
-      <c r="D29" t="s">
-        <v>45</v>
-      </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1067,13 +1070,13 @@
         <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1081,16 +1084,16 @@
         <v>45080</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>